<commit_message>
fixed add class and add teacher
</commit_message>
<xml_diff>
--- a/lihket_students_upload_template.xlsx
+++ b/lihket_students_upload_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Eyu Erbelo</t>
+  </si>
+  <si>
+    <t>Samuel Ayalew</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Ayalew Bikago</t>
   </si>
 </sst>
 </file>
@@ -884,7 +893,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,7 +941,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>251922692328</v>
+        <v>251920864496</v>
       </c>
       <c r="E2">
         <v>9</v>
@@ -941,7 +950,7 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>251994288422</v>
+        <v>251920864496</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -964,11 +973,31 @@
         <v>12</v>
       </c>
       <c r="H3">
-        <v>251917186899</v>
+        <v>251920864496</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>251931653440</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>251931653440</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1"/>

</xml_diff>